<commit_message>
stable with shinyjs hide button
</commit_message>
<xml_diff>
--- a/Available_datasets.xlsx
+++ b/Available_datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wm5wt/Desktop/LOCAL_cache/PlaqView/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDD11B5-32A8-5B4D-BE0D-90DA57E28F56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B1D781-CE1A-A948-8809-D74F34C865FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8860" yWindow="620" windowWidth="19940" windowHeight="16940" xr2:uid="{5C0CB6DF-74F5-E84F-91BF-65048458DE00}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Year</t>
   </si>
@@ -57,12 +57,6 @@
     <t>4 Patients</t>
   </si>
   <si>
-    <t>TEST #1</t>
-  </si>
-  <si>
-    <t>TEST #2</t>
-  </si>
-  <si>
     <t>DataID</t>
   </si>
   <si>
@@ -72,10 +66,28 @@
     <t>Test_1</t>
   </si>
   <si>
-    <t>Test_2</t>
-  </si>
-  <si>
     <t>Authors</t>
+  </si>
+  <si>
+    <t>Tissue</t>
+  </si>
+  <si>
+    <t>Place Holder</t>
+  </si>
+  <si>
+    <t>Future Datasets Will Appear Here</t>
+  </si>
+  <si>
+    <t>Check Back!</t>
+  </si>
+  <si>
+    <t>Will Be Coming in Late March</t>
+  </si>
+  <si>
+    <t>Coronary Artery</t>
+  </si>
+  <si>
+    <t>Multiple</t>
   </si>
 </sst>
 </file>
@@ -434,17 +446,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAE4BB4F-B325-9D4C-92D3-781BA71EF3E2}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -459,13 +474,16 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
-        <v>12</v>
+      <c r="H1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -482,32 +500,33 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
-        <v>13</v>
+      <c r="H2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>2077</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4">
-        <v>2077</v>
-      </c>
-      <c r="G4" t="s">
         <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
unlimited colors using rcolorbrewer extension
</commit_message>
<xml_diff>
--- a/Available_datasets.xlsx
+++ b/Available_datasets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wm5wt/Desktop/LOCAL_cache/PlaqView/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB13FC23-53F3-6244-A922-62F48AE3A54F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227A09E0-4E63-4049-8ECF-43C43EDD5EDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2800" yWindow="700" windowWidth="19940" windowHeight="16940" xr2:uid="{5C0CB6DF-74F5-E84F-91BF-65048458DE00}"/>
   </bookViews>
@@ -477,13 +477,13 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="33.33203125" customWidth="1"/>
-    <col min="4" max="4" width="35.5" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
tryin to speed it up and minor changes to UI
</commit_message>
<xml_diff>
--- a/Available_datasets.xlsx
+++ b/Available_datasets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wm5wt/Desktop/LOCAL_cache/PlaqView/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227A09E0-4E63-4049-8ECF-43C43EDD5EDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0BB72E-2B5A-6146-8065-EAAA6D1A0D0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="700" windowWidth="19940" windowHeight="16940" xr2:uid="{5C0CB6DF-74F5-E84F-91BF-65048458DE00}"/>
+    <workbookView xWindow="8860" yWindow="540" windowWidth="17400" windowHeight="16940" xr2:uid="{5C0CB6DF-74F5-E84F-91BF-65048458DE00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Year</t>
   </si>
@@ -94,13 +94,19 @@
   </si>
   <si>
     <t>CEL-Seq2</t>
+  </si>
+  <si>
+    <t>Carotid Endarterectomy</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -110,27 +116,40 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF222222"/>
-      <name val="Helvetica Neue"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -154,12 +173,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,109 +513,209 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAE4BB4F-B325-9D4C-92D3-781BA71EF3E2}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="C12" activeCellId="1" sqref="A4:XFD4 C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="33.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="17.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="13" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" s="8" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="1">
         <v>2019</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="4">
         <v>9798</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
         <v>2021</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="5">
         <v>6191</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="1" t="s">
         <v>13</v>
       </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="6"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H32" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
stable upload with pan et al
</commit_message>
<xml_diff>
--- a/Available_datasets.xlsx
+++ b/Available_datasets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wm5wt/Desktop/LOCAL_cache/PlaqView/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0BB72E-2B5A-6146-8065-EAAA6D1A0D0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C422364-5F8C-744F-A065-3843BA18A84A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8860" yWindow="540" windowWidth="17400" windowHeight="16940" xr2:uid="{5C0CB6DF-74F5-E84F-91BF-65048458DE00}"/>
+    <workbookView xWindow="1640" yWindow="1060" windowWidth="19920" windowHeight="16940" xr2:uid="{5C0CB6DF-74F5-E84F-91BF-65048458DE00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Year</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Tissue</t>
   </si>
   <si>
-    <t>Coronary Artery</t>
-  </si>
-  <si>
     <t>Slender_2021</t>
   </si>
   <si>
@@ -96,10 +93,31 @@
     <t>CEL-Seq2</t>
   </si>
   <si>
-    <t>Carotid Endarterectomy</t>
+    <t>Pan et al.</t>
+  </si>
+  <si>
+    <t>Circulation</t>
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>3 Patients</t>
+  </si>
+  <si>
+    <t>Pan_2020</t>
+  </si>
+  <si>
+    <t>Carotid Plaque</t>
+  </si>
+  <si>
+    <t>Coronary Artery Explant</t>
+  </si>
+  <si>
+    <t>Carotid Artery</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1161/CIRCULATIONAHA.120.048378</t>
   </si>
 </sst>
 </file>
@@ -516,7 +534,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" activeCellId="1" sqref="A4:XFD4 C12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,8 +542,10 @@
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="2" max="2" width="17.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="2"/>
-    <col min="4" max="4" width="13" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="42" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="2"/>
+    <col min="6" max="6" width="22.1640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="8" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
@@ -548,13 +568,13 @@
         <v>11</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>8</v>
@@ -562,7 +582,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -577,7 +597,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>7</v>
@@ -586,7 +606,7 @@
         <v>9798</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>9</v>
@@ -594,10 +614,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1">
         <v>2021</v>
@@ -609,29 +629,52 @@
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" s="5">
         <v>6191</v>
       </c>
       <c r="I3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="6"/>
-      <c r="J4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="6">
+        <v>8867</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H5" s="6"/>

</xml_diff>

<commit_message>
updated read me and drug panel
</commit_message>
<xml_diff>
--- a/Available_datasets.xlsx
+++ b/Available_datasets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wm5wt/Desktop/LOCAL_cache/PlaqView/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C422364-5F8C-744F-A065-3843BA18A84A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF331C5C-364A-D04E-8BC1-C0A4E6F0FF6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="1060" windowWidth="19920" windowHeight="16940" xr2:uid="{5C0CB6DF-74F5-E84F-91BF-65048458DE00}"/>
+    <workbookView xWindow="0" yWindow="1060" windowWidth="17820" windowHeight="16940" xr2:uid="{5C0CB6DF-74F5-E84F-91BF-65048458DE00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Year</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Slender_2021</t>
   </si>
   <si>
-    <t>Slender et al.</t>
-  </si>
-  <si>
     <t>Wirka et al.</t>
   </si>
   <si>
@@ -108,16 +105,25 @@
     <t>Pan_2020</t>
   </si>
   <si>
-    <t>Carotid Plaque</t>
-  </si>
-  <si>
-    <t>Coronary Artery Explant</t>
-  </si>
-  <si>
-    <t>Carotid Artery</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1161/CIRCULATIONAHA.120.048378</t>
+  </si>
+  <si>
+    <t>Coronary Artery</t>
+  </si>
+  <si>
+    <t>Carotid Artery Plaque</t>
+  </si>
+  <si>
+    <t>Procedure</t>
+  </si>
+  <si>
+    <t>Endarterectomy</t>
+  </si>
+  <si>
+    <t>Transplant</t>
+  </si>
+  <si>
+    <t>Slenders et al.</t>
   </si>
 </sst>
 </file>
@@ -531,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAE4BB4F-B325-9D4C-92D3-781BA71EF3E2}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,11 +550,11 @@
     <col min="3" max="3" width="10.83203125" style="2"/>
     <col min="4" max="4" width="42" style="2" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="2"/>
-    <col min="6" max="6" width="22.1640625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="6" max="7" width="22.1640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="8" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
@@ -568,21 +574,24 @@
         <v>11</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -597,168 +606,177 @@
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4">
+      <c r="I2" s="4">
         <v>9798</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="J2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1">
         <v>2021</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="5">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="5">
         <v>6191</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="C4" s="2">
         <v>2020</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="6">
+        <v>8867</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="6">
-        <v>8867</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H20" s="6"/>
-    </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H21" s="6"/>
-    </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H22" s="6"/>
-    </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H24" s="6"/>
-    </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H25" s="6"/>
-    </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H26" s="6"/>
-    </row>
-    <row r="27" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H27" s="6"/>
-    </row>
-    <row r="28" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H28" s="6"/>
-    </row>
-    <row r="29" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H29" s="6"/>
-    </row>
-    <row r="30" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H30" s="6"/>
-    </row>
-    <row r="31" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H31" s="6"/>
-    </row>
-    <row r="32" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H32" s="6"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I22" s="6"/>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I31" s="6"/>
+    </row>
+    <row r="32" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I32" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
unstable as of yet, just a check point for today
</commit_message>
<xml_diff>
--- a/Available_datasets.xlsx
+++ b/Available_datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wm5wt/Desktop/LOCAL_cache/PlaqView/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF331C5C-364A-D04E-8BC1-C0A4E6F0FF6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2965AF-2EB4-E948-8B4B-0D51109BF957}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1060" windowWidth="17820" windowHeight="16940" xr2:uid="{5C0CB6DF-74F5-E84F-91BF-65048458DE00}"/>
   </bookViews>
@@ -540,7 +540,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
removed wang et all completely
too small, 188 cells only and most tools cant run it
</commit_message>
<xml_diff>
--- a/Available_datasets.xlsx
+++ b/Available_datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wm5wt/My Drive/PlaqView_Master/PlaqView/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19010CE3-4FF5-964D-8C52-E885C1457778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EFD04F-A7A1-E243-831B-6C7A1484BE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5020" yWindow="500" windowWidth="20580" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
   <si>
     <t>Journal</t>
   </si>
@@ -225,31 +225,7 @@
     <t>12-18-21</t>
   </si>
   <si>
-    <t>Wang et al.</t>
-  </si>
-  <si>
-    <t>Cardiovascular Research</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1093/cvr/cvab347</t>
-  </si>
-  <si>
-    <t>Medial Aorta Layer and Plaque</t>
-  </si>
-  <si>
-    <t>Healthy vs Plaque Aortic SMC</t>
-  </si>
-  <si>
-    <t>ApoeE KO mice</t>
-  </si>
-  <si>
-    <t>Wang_2021_mouse</t>
-  </si>
-  <si>
     <t>https://academic.oup.com/ehjopen/advance-article/doi/10.1093/ehjopen/oeab043/6472573</t>
-  </si>
-  <si>
-    <t>NexteraXT DNA Library</t>
   </si>
 </sst>
 </file>
@@ -606,7 +582,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="G12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -792,7 +768,7 @@
         <v>2021</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -1198,42 +1174,17 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="5">
-        <v>2021</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="I12" s="5">
-        <v>188</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="L12" t="s">
-        <v>65</v>
-      </c>
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -28889,12 +28840,11 @@
     <hyperlink ref="D9" r:id="rId1" xr:uid="{39C72426-9689-4C4A-ADBC-FCF0559EE6A3}"/>
     <hyperlink ref="D10" r:id="rId2" xr:uid="{141F7345-D0DC-164A-BEA2-307B86915AAA}"/>
     <hyperlink ref="D11" r:id="rId3" xr:uid="{00CB8400-A1A4-5545-BA13-501386CB0FE1}"/>
-    <hyperlink ref="D12" r:id="rId4" xr:uid="{B3A96F28-0F78-5844-A53D-AB968CA95826}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>